<commit_message>
Modification 2 semaines au lieu de 2j quand on emprunte un livre
</commit_message>
<xml_diff>
--- a/Doc/Tasks/tasks.xlsx
+++ b/Doc/Tasks/tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -712,7 +712,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -756,6 +756,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1589,7 +1590,7 @@
   <dimension ref="C2:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1840,7 +1841,7 @@
     </row>
     <row r="32" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="8"/>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="27" t="s">
         <v>124</v>
       </c>
       <c r="F32" s="13"/>

</xml_diff>

<commit_message>
Design des tableaux refait
Faire une demande d'emprunt, mis à 2 semaines de base

Annuler une demande d'emprunt

Pouvoir accepter les demandes d'emprunt: en cours
</commit_message>
<xml_diff>
--- a/Doc/Tasks/tasks.xlsx
+++ b/Doc/Tasks/tasks.xlsx
@@ -712,7 +712,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -757,6 +757,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1589,8 +1590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C636A263-C7DD-4A9F-B724-027C5C4ADC20}">
   <dimension ref="C2:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1851,7 +1852,7 @@
     </row>
     <row r="33" spans="3:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C33" s="8"/>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="27" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1911,7 +1912,7 @@
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C44" s="8"/>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="28" t="s">
         <v>128</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Replace sur new pc
</commit_message>
<xml_diff>
--- a/Doc/Tasks/tasks.xlsx
+++ b/Doc/Tasks/tasks.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Task" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr autoRecover="0"/>
+  <fileRecoveryPr autoRecover="0" repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="159">
   <si>
     <t>Nom de la class</t>
   </si>
@@ -447,6 +447,57 @@
   </si>
   <si>
     <t>Accepter et refuser des demandes d'emprunt</t>
+  </si>
+  <si>
+    <t>Déplacer le bouton disconnect du mode super admin comme pour le normal</t>
+  </si>
+  <si>
+    <t>Système</t>
+  </si>
+  <si>
+    <t>Niveau d'accès: liste déroulante des string</t>
+  </si>
+  <si>
+    <t>Ne rien faire si on save qqch mais on modifie rien</t>
+  </si>
+  <si>
+    <t>Demander confirmation lorsqu'on supprime qqch</t>
+  </si>
+  <si>
+    <t>Réduire la taille des icônes</t>
+  </si>
+  <si>
+    <t>Mettre le nom des biblio au lieu de leurs id en liste déroulante</t>
+  </si>
+  <si>
+    <t>Pouvoir trier la liste d'une table suivant une colonne</t>
+  </si>
+  <si>
+    <t>Changer la couleur Admin: orange, SuperAdmin: rouge</t>
+  </si>
+  <si>
+    <t>Si on peut pas save/delete un champs, le disabled</t>
+  </si>
+  <si>
+    <t>Séparer en trois sections le panel super admin</t>
+  </si>
+  <si>
+    <t>Page: add les &gt;&gt; et &lt;&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expiration de token </t>
+  </si>
+  <si>
+    <t>Ne pas montrer le panel admin si on est log sur un compte 6&lt;</t>
+  </si>
+  <si>
+    <t>Enlever la création de compte</t>
+  </si>
+  <si>
+    <t>Enlever le bouton du panel admin sur la page principale</t>
+  </si>
+  <si>
+    <t>Faire une script qui génère le .jar, javadoc et delete les .zip dans git &gt;&gt; modifier le guide</t>
   </si>
 </sst>
 </file>
@@ -599,7 +650,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -704,6 +755,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -712,7 +783,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -758,6 +829,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1588,10 +1666,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C636A263-C7DD-4A9F-B724-027C5C4ADC20}">
-  <dimension ref="C2:G47"/>
+  <dimension ref="C2:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1811,6 +1889,14 @@
       </c>
       <c r="E24" s="16"/>
     </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="30">
+        <v>7</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>158</v>
+      </c>
+    </row>
     <row r="28" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="3:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F29" s="10" t="s">
@@ -1882,56 +1968,155 @@
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="28" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C40" s="8" t="s">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39"/>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D40" s="8"/>
-    </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C41" s="8"/>
-      <c r="D41" s="9" t="s">
-        <v>127</v>
-      </c>
+      <c r="D41" s="8"/>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C42" s="8"/>
       <c r="D42" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C43" s="8"/>
       <c r="D43" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C44" s="8"/>
-      <c r="D44" s="27" t="s">
-        <v>141</v>
+      <c r="D44" s="9" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C45" s="8"/>
-      <c r="D45" s="6" t="s">
-        <v>128</v>
+      <c r="D45" s="27" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C46" s="8"/>
       <c r="D46" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C47" s="8"/>
       <c r="D47" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C48" s="8"/>
+      <c r="D48" s="6" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="D51" s="28"/>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="28"/>
+      <c r="D52" s="29" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53" s="28"/>
+      <c r="D53" s="29" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C54" s="28"/>
+      <c r="D54" s="29" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C55" s="28"/>
+      <c r="D55" s="29" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="28"/>
+      <c r="D56" s="29" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57" s="28"/>
+      <c r="D57" s="29" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C58" s="28"/>
+      <c r="D58" s="29" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C59" s="28"/>
+      <c r="D59" s="29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="28"/>
+      <c r="D60" s="29" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C61" s="28"/>
+      <c r="D61" s="29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C62" s="28"/>
+      <c r="D62" s="29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C63" s="28"/>
+      <c r="D63" s="29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C64" s="28"/>
+      <c r="D64" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C65" s="28"/>
+      <c r="D65" s="29" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C66" s="28"/>
+      <c r="D66" s="29" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creation d'un script de création du jar et javadoc
</commit_message>
<xml_diff>
--- a/Doc/Tasks/tasks.xlsx
+++ b/Doc/Tasks/tasks.xlsx
@@ -494,13 +494,13 @@
     <t>Enlever la création de compte</t>
   </si>
   <si>
-    <t>Enlever le bouton du panel admin sur la page principale</t>
-  </si>
-  <si>
     <t>Faire une script qui génère le .jar, javadoc et delete les .zip dans git &gt;&gt; modifier le guide</t>
   </si>
   <si>
-    <t>Liate des user fait</t>
+    <t>Enlever le bouton du panel admin sur la page principale, ne le montrer qu'en étant connecté déjà en admin</t>
+  </si>
+  <si>
+    <t>Liste des user fait</t>
   </si>
 </sst>
 </file>
@@ -1672,13 +1672,13 @@
   <dimension ref="C2:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="9.140625" style="6"/>
-    <col min="4" max="4" width="80.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="99" style="6" customWidth="1"/>
     <col min="5" max="5" width="94.28515625" style="6" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="6"/>
     <col min="7" max="7" width="28.42578125" style="6" customWidth="1"/>
@@ -1897,7 +1897,7 @@
         <v>7</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2122,7 +2122,7 @@
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C66" s="28"/>
       <c r="D66" s="29" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finition des script .bat
Fix du .jar

Multiples ajouts sur le site
</commit_message>
<xml_diff>
--- a/Doc/Tasks/tasks.xlsx
+++ b/Doc/Tasks/tasks.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="164">
   <si>
     <t>Nom de la class</t>
   </si>
@@ -497,10 +497,22 @@
     <t>Faire une script qui génère le .jar, javadoc et delete les .zip dans git &gt;&gt; modifier le guide</t>
   </si>
   <si>
-    <t>Enlever le bouton du panel admin sur la page principale, ne le montrer qu'en étant connecté déjà en admin</t>
-  </si>
-  <si>
     <t>Liste des user fait</t>
+  </si>
+  <si>
+    <t>si le superadmin se log, il sera déjà log sur le panel superadmin</t>
+  </si>
+  <si>
+    <t>ajouter la date limite du livre avant de devoir le rendre sur liste des livres renter et partie admin</t>
+  </si>
+  <si>
+    <t>Faire un script pour faire une backup de la db</t>
+  </si>
+  <si>
+    <t>Laisser la ligne de création d'un livre même il n'y aucuns livres dans la biblio</t>
+  </si>
+  <si>
+    <t>Pouvoir switch entre les bibliothèque sans devoir se déconnecter avant</t>
   </si>
 </sst>
 </file>
@@ -1669,10 +1681,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C636A263-C7DD-4A9F-B724-027C5C4ADC20}">
-  <dimension ref="C2:G66"/>
+  <dimension ref="C2:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1953,7 +1965,7 @@
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C35" s="8"/>
-      <c r="D35" s="28" t="s">
+      <c r="D35" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1971,7 +1983,7 @@
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C38" s="8"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2082,11 +2094,11 @@
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C60" s="28"/>
-      <c r="D60" s="28" t="s">
+      <c r="D60" s="27" t="s">
         <v>151</v>
       </c>
       <c r="E60" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="3:5" x14ac:dyDescent="0.25">
@@ -2115,15 +2127,42 @@
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C65" s="28"/>
-      <c r="D65" s="29" t="s">
+      <c r="D65" s="27" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C66" s="28"/>
-      <c r="D66" s="29" t="s">
-        <v>158</v>
-      </c>
+      <c r="D66" s="27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C67" s="28"/>
+      <c r="D67" s="29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C68" s="28"/>
+      <c r="D68" s="29" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C69" s="28"/>
+      <c r="D69" s="27" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C70" s="28"/>
+      <c r="D70" s="27" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D71"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajout de mysql_import.bat pour importer facilement la db
</commit_message>
<xml_diff>
--- a/Doc/Tasks/tasks.xlsx
+++ b/Doc/Tasks/tasks.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="163">
   <si>
     <t>Nom de la class</t>
   </si>
@@ -495,9 +495,6 @@
   </si>
   <si>
     <t>Faire une script qui génère le .jar, javadoc et delete les .zip dans git &gt;&gt; modifier le guide</t>
-  </si>
-  <si>
-    <t>Liste des user fait</t>
   </si>
   <si>
     <t>si le superadmin se log, il sera déjà log sur le panel superadmin</t>
@@ -1684,7 +1681,7 @@
   <dimension ref="C2:G71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2046,7 +2043,7 @@
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C52" s="28"/>
-      <c r="D52" s="29" t="s">
+      <c r="D52" s="27" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2097,13 +2094,11 @@
       <c r="D60" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="E60" s="29" t="s">
-        <v>158</v>
-      </c>
+      <c r="E60" s="29"/>
     </row>
     <row r="61" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C61" s="28"/>
-      <c r="D61" s="29" t="s">
+      <c r="D61" s="28" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2121,7 +2116,7 @@
     </row>
     <row r="64" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C64" s="28"/>
-      <c r="D64" s="29" t="s">
+      <c r="D64" s="27" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2134,31 +2129,31 @@
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C66" s="28"/>
       <c r="D66" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C67" s="28"/>
       <c r="D67" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C68" s="28"/>
-      <c r="D68" s="29" t="s">
-        <v>161</v>
+      <c r="D68" s="27" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C69" s="28"/>
       <c r="D69" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C70" s="28"/>
       <c r="D70" s="27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modification dans le web: Panel administrateur et url rest dans Utils.class.php
</commit_message>
<xml_diff>
--- a/Doc/Tasks/tasks.xlsx
+++ b/Doc/Tasks/tasks.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -795,7 +795,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -846,6 +846,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1680,8 +1683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C636A263-C7DD-4A9F-B724-027C5C4ADC20}">
   <dimension ref="C2:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1860,7 +1863,7 @@
       <c r="C20" s="14">
         <v>8</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="32" t="s">
         <v>110</v>
       </c>
       <c r="E20" s="17" t="s">
@@ -2067,13 +2070,13 @@
     </row>
     <row r="56" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C56" s="28"/>
-      <c r="D56" s="29" t="s">
+      <c r="D56" s="27" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C57" s="28"/>
-      <c r="D57" s="29" t="s">
+      <c r="D57" s="27" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2098,7 +2101,7 @@
     </row>
     <row r="61" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C61" s="28"/>
-      <c r="D61" s="28" t="s">
+      <c r="D61" s="27" t="s">
         <v>152</v>
       </c>
     </row>

</xml_diff>